<commit_message>
Share Account 5 testcases, Teller/Cash 10 testcases
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/4106-CREATACTIVEGROUP-WITHCLIENTATTACHED-EDIT.xlsx
+++ b/Mifos Automation Excels/Client/4106-CREATACTIVEGROUP-WITHCLIENTATTACHED-EDIT.xlsx
@@ -55,9 +55,6 @@
     <t>EditGroupname</t>
   </si>
   <si>
-    <t>96Group</t>
-  </si>
-  <si>
     <t>ClickOnEditSubmit</t>
   </si>
   <si>
@@ -83,6 +80,9 @@
   </si>
   <si>
     <t>VerifyClientCreated</t>
+  </si>
+  <si>
+    <t>6014Group</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -549,15 +549,15 @@
     </row>
     <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="6">
         <v>42005</v>
@@ -565,15 +565,15 @@
     </row>
     <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>7</v>
@@ -600,12 +600,12 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -622,7 +622,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -637,15 +637,15 @@
         <v>8</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>